<commit_message>
Fixed footer changes issues
</commit_message>
<xml_diff>
--- a/Resources/TestData/qat01.xlsx
+++ b/Resources/TestData/qat01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="260">
   <si>
     <t>TC_NO</t>
   </si>
@@ -118,18 +118,6 @@
     <t>Ftrfrank1+automationtest01@gmail.com</t>
   </si>
   <si>
-    <t>Oct 17, 2017</t>
-  </si>
-  <si>
-    <t>10/17/17 - 11/16/17</t>
-  </si>
-  <si>
-    <t>$719.95</t>
-  </si>
-  <si>
-    <t>Oct 11, 2017</t>
-  </si>
-  <si>
     <t>TC04</t>
   </si>
   <si>
@@ -421,9 +409,6 @@
     <t>https://qat01.frontier.com/shop/frontier-secure</t>
   </si>
   <si>
-    <t>https://qat01.frontier.com/corporate/movers</t>
-  </si>
-  <si>
     <t>https://qat01.frontier.com/resources/discount-programs</t>
   </si>
   <si>
@@ -475,24 +460,12 @@
     <t>http://investor.frontier.com/</t>
   </si>
   <si>
-    <t>http://investor.frontier.com/releases.cfm</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/careers/overview</t>
-  </si>
-  <si>
-    <t>https://qat01.frontier.com/corporate/suppliers</t>
-  </si>
-  <si>
     <t>https://frontier.com/corporate/news/home</t>
   </si>
   <si>
     <t>https://qat01.frontier.com/makingadifference</t>
   </si>
   <si>
-    <t>https://qat01.frontier.com/corporate/pif/public-inspection-files</t>
-  </si>
-  <si>
     <t>005_CC_.COM_Desktop_NSS_Res_Footers_FrontierSites</t>
   </si>
   <si>
@@ -797,6 +770,39 @@
   </si>
   <si>
     <t>https://qat01.frontier.com/resources/movers</t>
+  </si>
+  <si>
+    <t>https://qat01.frontier.com/corporate/news/home</t>
+  </si>
+  <si>
+    <t>https://frontier.silkroad.com/epostings/</t>
+  </si>
+  <si>
+    <t>https://qat01.frontier.com/corporate/company/supplier</t>
+  </si>
+  <si>
+    <t>https://qat01.frontier.com/corporate/responsibility/inspection-files/home</t>
+  </si>
+  <si>
+    <t>Zipcode1</t>
+  </si>
+  <si>
+    <t>75024</t>
+  </si>
+  <si>
+    <t>Dec 13, 2017</t>
+  </si>
+  <si>
+    <t>12/13/17 - 1/12/18</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>$90.98</t>
+  </si>
+  <si>
+    <t>Jan 8, 2018</t>
   </si>
 </sst>
 </file>
@@ -1324,11 +1330,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,22 +1488,22 @@
         <v>27</v>
       </c>
       <c r="H3" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="I3" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>32</v>
-      </c>
       <c r="K3" s="26" t="s">
-        <v>33</v>
+        <v>257</v>
       </c>
       <c r="L3" s="26" t="s">
-        <v>33</v>
+        <v>258</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>34</v>
+        <v>259</v>
       </c>
       <c r="N3" s="26"/>
       <c r="O3" s="26"/>
@@ -1510,10 +1516,10 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>23</v>
@@ -1537,16 +1543,16 @@
       <c r="L4" s="26"/>
       <c r="M4" s="26"/>
       <c r="N4" s="26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="O4" s="26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="P4" s="26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="R4" s="26"/>
       <c r="S4" s="26"/>
@@ -1555,10 +1561,10 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>23</v>
@@ -1592,10 +1598,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>23</v>
@@ -1623,19 +1629,19 @@
       <c r="P6" s="26"/>
       <c r="Q6" s="26"/>
       <c r="R6" s="26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="S6" s="26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U6" s="26"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>23</v>
@@ -1665,16 +1671,16 @@
       <c r="R7" s="26"/>
       <c r="S7" s="26"/>
       <c r="T7" s="33" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="U7" s="26"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>23</v>
@@ -1708,16 +1714,16 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>25</v>
@@ -1745,10 +1751,10 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>23</v>
@@ -1760,7 +1766,7 @@
         <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>27</v>
@@ -1779,15 +1785,15 @@
       <c r="S10" s="26"/>
       <c r="T10" s="33"/>
       <c r="U10" s="34" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>23</v>
@@ -1799,10 +1805,10 @@
         <v>25</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -1821,10 +1827,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>23</v>
@@ -1902,11 +1908,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BM17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="AI11" sqref="AI11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,7 +1950,7 @@
     <col min="31" max="31" width="44" style="29" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="39.7109375" style="29" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="39.7109375" style="29" customWidth="1"/>
-    <col min="34" max="34" width="59.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="69.5703125" style="29" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="23.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="21.42578125" style="29" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="28.7109375" style="29" bestFit="1" customWidth="1"/>
@@ -1991,7 +1997,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -2000,222 +2006,222 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="P1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="Q1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="T1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="U1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="V1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="W1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="AA1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="AB1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AC1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AD1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AE1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AF1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AI1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AK1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AL1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AM1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AN1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AR1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AS1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AT1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AU1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AR1" s="12" t="s">
+      <c r="AV1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AS1" s="12" t="s">
+      <c r="AW1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="AT1" s="12" t="s">
+      <c r="AX1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="AU1" s="12" t="s">
+      <c r="AY1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AW1" s="12" t="s">
+      <c r="BA1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="AX1" s="12" t="s">
+      <c r="BB1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AY1" s="12" t="s">
+      <c r="BC1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BD1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="BA1" s="14" t="s">
+      <c r="BE1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="BB1" s="7" t="s">
+      <c r="BF1" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="BG1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BH1" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="BE1" s="9" t="s">
+      <c r="BI1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="BF1" s="9" t="s">
+      <c r="BJ1" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BK1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="BH1" s="14" t="s">
+      <c r="BL1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="BI1" s="14" t="s">
+      <c r="BM1" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="BJ1" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="BK1" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="BL1" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BM1" s="8" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="I2" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="26" t="s">
+      <c r="J2" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="K2" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="L2" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="35" t="s">
-        <v>257</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="T2" s="26"/>
       <c r="U2" s="26"/>
@@ -2269,13 +2275,13 @@
         <v>21</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>24</v>
@@ -2291,22 +2297,22 @@
       <c r="L3" s="26"/>
       <c r="M3" s="26"/>
       <c r="N3" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="S3" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="T3" s="26"/>
       <c r="U3" s="26"/>
@@ -2360,13 +2366,13 @@
         <v>28</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>24</v>
@@ -2388,25 +2394,25 @@
       <c r="R4" s="26"/>
       <c r="S4" s="26"/>
       <c r="T4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="AA4" s="26"/>
       <c r="AB4" s="26"/>
@@ -2450,16 +2456,16 @@
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
@@ -2488,28 +2494,28 @@
       <c r="Y5" s="26"/>
       <c r="Z5" s="26"/>
       <c r="AA5" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
+      </c>
+      <c r="AC5" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD5" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE5" s="35" t="s">
+        <v>251</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
+      </c>
+      <c r="AH5" s="35" t="s">
+        <v>252</v>
       </c>
       <c r="AI5" s="26"/>
       <c r="AJ5" s="26"/>
@@ -2545,16 +2551,16 @@
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
@@ -2591,31 +2597,31 @@
       <c r="AG6" s="26"/>
       <c r="AH6" s="26"/>
       <c r="AI6" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="AK6" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN6" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="AQ6" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="AR6" s="26"/>
       <c r="AS6" s="26"/>
@@ -2642,16 +2648,16 @@
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
@@ -2697,28 +2703,28 @@
       <c r="AP7" s="26"/>
       <c r="AQ7" s="26"/>
       <c r="AR7" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="AS7" s="15" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AT7" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AU7" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="AV7" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="AW7" s="15" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="AX7" s="15" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="AY7" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="AZ7" s="26"/>
       <c r="BA7" s="26"/>
@@ -2737,16 +2743,16 @@
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>24</v>
@@ -2800,7 +2806,7 @@
       <c r="AX8" s="26"/>
       <c r="AY8" s="26"/>
       <c r="AZ8" s="15" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="BA8" s="26"/>
       <c r="BB8" s="26"/>
@@ -2818,16 +2824,16 @@
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>24</v>
@@ -2882,7 +2888,7 @@
       <c r="AY9" s="26"/>
       <c r="AZ9" s="26"/>
       <c r="BA9" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="BB9" s="26"/>
       <c r="BC9" s="26"/>
@@ -2899,16 +2905,16 @@
     </row>
     <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>24</v>
@@ -2964,7 +2970,7 @@
       <c r="AZ10" s="26"/>
       <c r="BA10" s="26"/>
       <c r="BB10" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="BC10" s="26"/>
       <c r="BD10" s="26"/>
@@ -2980,16 +2986,16 @@
     </row>
     <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>24</v>
@@ -3046,7 +3052,7 @@
       <c r="BA11" s="26"/>
       <c r="BB11" s="26"/>
       <c r="BC11" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="BD11" s="26"/>
       <c r="BE11" s="26"/>
@@ -3061,16 +3067,16 @@
     </row>
     <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>24</v>
@@ -3128,7 +3134,7 @@
       <c r="BB12" s="26"/>
       <c r="BC12" s="26"/>
       <c r="BD12" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="BE12" s="26"/>
       <c r="BF12" s="26"/>
@@ -3142,16 +3148,16 @@
     </row>
     <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
@@ -3210,10 +3216,10 @@
       <c r="BC13" s="26"/>
       <c r="BD13" s="26"/>
       <c r="BE13" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="BF13" s="26" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="BG13" s="26"/>
       <c r="BH13" s="26"/>
@@ -3225,16 +3231,16 @@
     </row>
     <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>24</v>
@@ -3295,7 +3301,7 @@
       <c r="BE14" s="26"/>
       <c r="BF14" s="26"/>
       <c r="BG14" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="BH14" s="26"/>
       <c r="BI14" s="26"/>
@@ -3306,16 +3312,16 @@
     </row>
     <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>24</v>
@@ -3377,10 +3383,10 @@
       <c r="BF15" s="26"/>
       <c r="BG15" s="26"/>
       <c r="BH15" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="BI15" s="26" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="BJ15" s="26"/>
       <c r="BK15" s="26"/>
@@ -3389,16 +3395,16 @@
     </row>
     <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>24</v>
@@ -3462,26 +3468,26 @@
       <c r="BH16" s="26"/>
       <c r="BI16" s="26"/>
       <c r="BJ16" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="BK16" s="26" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="BL16" s="26"/>
       <c r="BM16" s="26"/>
     </row>
     <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>24</v>
@@ -3547,10 +3553,10 @@
       <c r="BJ17" s="26"/>
       <c r="BK17" s="26"/>
       <c r="BL17" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="BM17" s="26" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3618,13 +3624,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,14 +3643,15 @@
     <col min="6" max="6" width="21.7109375" style="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.7109375" style="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="6.7109375" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="6.7109375" style="24"/>
+    <col min="9" max="9" width="9.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="6.7109375" style="24" customWidth="1"/>
+    <col min="17" max="16384" width="6.7109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -3655,7 +3662,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>3</v>
@@ -3670,27 +3677,30 @@
         <v>6</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>203</v>
+        <v>253</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>24</v>
@@ -3701,27 +3711,30 @@
       <c r="G2" s="23"/>
       <c r="H2" s="21"/>
       <c r="I2" s="22" t="s">
-        <v>207</v>
+        <v>254</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>24</v>
@@ -3734,19 +3747,20 @@
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="20"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>24</v>
@@ -3755,7 +3769,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>27</v>
@@ -3763,19 +3777,20 @@
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>24</v>
@@ -3788,19 +3803,20 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="20"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>24</v>
@@ -3813,19 +3829,20 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="20"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>24</v>
@@ -3838,19 +3855,20 @@
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="20"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>24</v>
@@ -3863,19 +3881,20 @@
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="20"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>24</v>
@@ -3888,19 +3907,20 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="20"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>24</v>
@@ -3913,6 +3933,7 @@
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3931,10 +3952,10 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3973,7 +3994,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -3982,57 +4003,57 @@
         <v>4</v>
       </c>
       <c r="G1" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="S1" s="31" t="s">
         <v>221</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>224</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="S1" s="31" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>24</v>
@@ -4041,7 +4062,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
@@ -4055,13 +4076,13 @@
         <v>21</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>24</v>
@@ -4071,7 +4092,7 @@
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I3" s="26"/>
       <c r="J3" s="26"/>
@@ -4090,13 +4111,13 @@
         <v>28</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>24</v>
@@ -4107,7 +4128,7 @@
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
       <c r="I4" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J4" s="26"/>
       <c r="K4" s="26"/>
@@ -4122,16 +4143,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>24</v>
@@ -4143,7 +4164,7 @@
       <c r="H5" s="26"/>
       <c r="I5" s="26"/>
       <c r="J5" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
@@ -4157,16 +4178,16 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>24</v>
@@ -4179,7 +4200,7 @@
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
       <c r="K6" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
@@ -4192,16 +4213,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>24</v>
@@ -4214,8 +4235,8 @@
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="2" t="s">
-        <v>132</v>
+      <c r="L7" s="35" t="s">
+        <v>248</v>
       </c>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
@@ -4227,16 +4248,16 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>24</v>
@@ -4260,16 +4281,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>24</v>
@@ -4293,16 +4314,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>24</v>
@@ -4326,16 +4347,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E11" s="27" t="s">
         <v>24</v>
@@ -4350,7 +4371,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="2" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -4361,16 +4382,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E12" s="27" t="s">
         <v>24</v>
@@ -4386,7 +4407,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -4396,16 +4417,16 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E13" s="27" t="s">
         <v>24</v>
@@ -4422,7 +4443,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="17" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -4431,16 +4452,16 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E14" s="27" t="s">
         <v>24</v>
@@ -4458,7 +4479,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -4466,16 +4487,16 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E15" s="27" t="s">
         <v>24</v>
@@ -4494,23 +4515,23 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E16" s="27" t="s">
         <v>24</v>
@@ -4530,22 +4551,22 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E17" s="27" t="s">
         <v>24</v>
@@ -4566,7 +4587,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4607,40 +4628,40 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>

</xml_diff>

<commit_message>
fixed css selector for Support
</commit_message>
<xml_diff>
--- a/Resources/TestData/qat01.xlsx
+++ b/Resources/TestData/qat01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Robot\DotCom\Resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A254A974-0ADC-41B0-A5D7-DC0923041748}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C30681-5335-4948-B0EF-06E47E2E9BC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REG" sheetId="1" r:id="rId1"/>
@@ -1161,11 +1161,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:C11"/>
+      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5351,7 +5351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>